<commit_message>
Updata khoa, bo mon
</commit_message>
<xml_diff>
--- a/data_diem.xlsx
+++ b/data_diem.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>Năm học</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Nguyễn Đắc Huy</t>
+  </si>
+  <si>
+    <t>C+</t>
   </si>
   <si>
     <t>Huyền Trang</t>
@@ -597,7 +600,7 @@
         <v>20</v>
       </c>
       <c r="E11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -606,13 +609,13 @@
         <v>5</v>
       </c>
       <c r="H11">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I11">
-        <v>7.3</v>
+        <v>6.5</v>
       </c>
       <c r="J11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -623,7 +626,7 @@
         <v>1221050420</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>

</xml_diff>